<commit_message>
Lower Flow regime converged much better and ran with new SRP case
</commit_message>
<xml_diff>
--- a/data/Results/Profiles.xlsx
+++ b/data/Results/Profiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\364265\Documents\git\Absorption_Column\data\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBCC9EFA-9F18-443C-8CE1-6AFCE0C2C497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{027A3B35-821D-405C-B67A-1D1FE3B31A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="772" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="23040" windowHeight="12204" tabRatio="772" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fl" sheetId="23" r:id="rId1"/>

</xml_diff>